<commit_message>
Improve structure and ui. Add ability to delete break and to edit student's comment
</commit_message>
<xml_diff>
--- a/server/template.xlsx
+++ b/server/template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>login</t>
   </si>
@@ -28,7 +28,10 @@
     <t>apolline.couturier-gauducheau@epitech.eu</t>
   </si>
   <si>
-    <t>16:20 -&gt; 16:40</t>
+    <t/>
+  </si>
+  <si>
+    <t>AM: Bon investissement, problème de visualisation des boucles</t>
   </si>
   <si>
     <t>axel.lopez@epitech.eu</t>
@@ -37,13 +40,10 @@
     <t>baptiste.vezien@epitech.eu</t>
   </si>
   <si>
-    <t>17:00 -&gt; 17:04</t>
-  </si>
-  <si>
     <t>cleophee.itier@epitech.eu</t>
   </si>
   <si>
-    <t>16:48 -&gt; 16:51</t>
+    <t>11:15 -&gt; 11:16</t>
   </si>
   <si>
     <t>damien.carrere@epitech.eu</t>
@@ -52,41 +52,25 @@
     <t>dean.artigaut@epitech.eu</t>
   </si>
   <si>
-    <t>15:44 -&gt; 15:56
-17:00 -&gt; 17:10
-17:39 -&gt; 17:40</t>
-  </si>
-  <si>
     <t>elhadj-makan.traore@epitech.eu</t>
   </si>
   <si>
-    <t>14:55 -&gt; 15:03
-16:26 -&gt; 16:40
-17:00 -&gt; 17:09</t>
-  </si>
-  <si>
     <t>enzo.bakri@epitech.eu</t>
   </si>
   <si>
     <t>esteban.juan@epitech.eu</t>
   </si>
   <si>
-    <t>16:26 -&gt; 16:30</t>
-  </si>
-  <si>
     <t>florian.wilk@epitech.eu</t>
   </si>
   <si>
-    <t>15:30 -&gt; 15:46
-16:58 -&gt; 17:06
-17:19 -&gt; 17:24</t>
+    <t>11:44 -&gt; 11:50</t>
   </si>
   <si>
     <t>franck.bellocq@epitech.eu</t>
   </si>
   <si>
-    <t>15:09 -&gt; 15:17
-16:58 -&gt; 17:07</t>
+    <t>10:21 -&gt; 10:34</t>
   </si>
   <si>
     <t>jinyang.zou@epitech.eu</t>
@@ -101,24 +85,21 @@
     <t>lohan.delomenie@epitech.eu</t>
   </si>
   <si>
-    <t>16:28 -&gt; 16:46
-17:00 -&gt; 17:14</t>
+    <t>09:41 -&gt; 09:43
+09:46 -&gt; 09:54
+10:21 -&gt; 10:34
+10:40 -&gt; 10:53</t>
   </si>
   <si>
     <t>luka.constantin@epitech.eu</t>
   </si>
   <si>
-    <t>15:29 -&gt; 15:57
-17:00 -&gt; 17:49</t>
+    <t>11:02 -&gt; 11:04</t>
   </si>
   <si>
     <t>mathias.cassonnet@epitech.eu</t>
   </si>
   <si>
-    <t>16:24 -&gt; 16:40
-17:01 -&gt; 17:09</t>
-  </si>
-  <si>
     <t>matthis.carle@epitech.eu</t>
   </si>
   <si>
@@ -128,30 +109,26 @@
     <t>nadir.allem@epitech.eu</t>
   </si>
   <si>
-    <t>14:32 -&gt; 14:33
-15:15 -&gt; 15:20
-16:58 -&gt; 17:06</t>
+    <t>10:10 -&gt; 10:12
+11:44 -&gt; 11:50</t>
   </si>
   <si>
     <t>nathan.frappier@epitech.eu</t>
   </si>
   <si>
-    <t>17:00 -&gt; 17:08</t>
-  </si>
-  <si>
     <t>nicolas.lapu@epitech.eu</t>
   </si>
   <si>
-    <t>16:00 -&gt; 16:08
-17:00 -&gt; 17:18</t>
+    <t>11:10 -&gt; 11:12
+11:12 -&gt; 11:12</t>
+  </si>
+  <si>
+    <t>AM: Bonne progression, des difficultés sur les caractères majuscules/minuscules qui a sût surmonter</t>
   </si>
   <si>
     <t>olivier.emiot@epitech.eu</t>
   </si>
   <si>
-    <t>16:56 -&gt; 16:56</t>
-  </si>
-  <si>
     <t>pierre-malko.denat@epitech.eu</t>
   </si>
   <si>
@@ -161,35 +138,30 @@
     <t>thomas.demonchaux@epitech.eu</t>
   </si>
   <si>
-    <t>14:32 -&gt; 14:34
-17:00 -&gt; 17:26</t>
+    <t>09:43 -&gt; 09:50</t>
   </si>
   <si>
     <t>thomas.labrousse@epitech.eu</t>
   </si>
   <si>
-    <t>15:29 -&gt; 15:59
-17:00 -&gt; 17:07</t>
+    <t>11:22 -&gt; 11:29</t>
   </si>
   <si>
     <t>valentin.erdozain@epitech.eu</t>
   </si>
   <si>
-    <t>17:08 -&gt; 17:49</t>
-  </si>
-  <si>
     <t>victor.miot@epitech.eu</t>
   </si>
   <si>
-    <t>15:09 -&gt; 15:16
-16:59 -&gt; 17:07</t>
+    <t>10:00 -&gt; 10:00
+10:22 -&gt; 10:34</t>
   </si>
   <si>
     <t>yann.marcotte@epitech.eu</t>
   </si>
   <si>
-    <t>15:25 -&gt; 15:29
-17:08 -&gt; 17:49</t>
+    <t>09:12 -&gt; 09:15
+10:34 -&gt; 10:37</t>
   </si>
 </sst>
 </file>
@@ -233,8 +205,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.2"/>
@@ -574,28 +546,28 @@
       </c>
     </row>
     <row r="2" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -618,212 +590,201 @@
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
     <row r="8" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
     <row r="19" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
     <row r="21" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
     <row r="23" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="24" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>40</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
     <row r="25" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
     <row r="26" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
     <row r="27" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C27" s="2"/>
     </row>
     <row r="28" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C28" s="2"/>
     </row>
     <row r="29" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>48</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
     <row r="30" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C30" s="2"/>
     </row>
     <row r="31" ht="60" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>46</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>